<commit_message>
manual guess kind of accurate
</commit_message>
<xml_diff>
--- a/assignment1/digit-feature-data/Numbers.xlsx
+++ b/assignment1/digit-feature-data/Numbers.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-35160" yWindow="900" windowWidth="28800" windowHeight="17600" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="440" yWindow="640" windowWidth="28800" windowHeight="17600" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="0" sheetId="3" r:id="rId1"/>
@@ -72,10 +72,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -98,13 +114,109 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -383,7 +495,7 @@
   <dimension ref="A1:K100"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:K16"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3077,6 +3189,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -3085,12 +3198,13 @@
   <dimension ref="A1:K100"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:K16"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="10" max="10" width="21.1640625" customWidth="1"/>
+    <col min="11" max="11" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -5779,6 +5893,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -5786,13 +5901,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:K16"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="J29" activeCellId="1" sqref="K10 J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="10" max="10" width="23" customWidth="1"/>
+    <col min="11" max="11" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -8481,6 +8597,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -8488,13 +8605,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView showRuler="0" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="10" max="10" width="19" customWidth="1"/>
+    <col min="11" max="11" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -11183,5 +11301,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Now process the hole balance
numbers with holes accuracy at 97.25%
</commit_message>
<xml_diff>
--- a/assignment1/digit-feature-data/Numbers.xlsx
+++ b/assignment1/digit-feature-data/Numbers.xlsx
@@ -132,8 +132,62 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -186,7 +240,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="103">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -211,6 +265,33 @@
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -235,6 +316,33 @@
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -513,7 +621,7 @@
   <dimension ref="A1:M100"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3860,7 +3968,7 @@
   <dimension ref="A1:M100"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection sqref="A1:J100"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7207,7 +7315,7 @@
   <dimension ref="A1:M100"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection sqref="A1:J100"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10554,7 +10662,7 @@
   <dimension ref="A1:M100"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>